<commit_message>
preparacao do sorteio pronta
</commit_message>
<xml_diff>
--- a/temp.xlsx
+++ b/temp.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\testes\loteriasServer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{401075A3-E760-4575-912F-A82120D946AA}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="12120" windowHeight="17430" xr2:uid="{21DE5BAD-0E6E-4206-8574-B64D9BE78428}"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="12120" windowHeight="17430"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -111,7 +110,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -458,16 +457,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D8607C3-F695-4A37-9843-965407CF7EAE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:AA25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView tabSelected="1" topLeftCell="B17" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4:E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="27.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="47.85546875" bestFit="1" customWidth="1"/>

</xml_diff>